<commit_message>
Onboarding Task for review
</commit_message>
<xml_diff>
--- a/Task1.xlsx
+++ b/Task1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7788AFB3-45EC-4E84-B56B-770A0531727A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3778B1FB-64F9-4A1F-99E6-7531E487455F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4080" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{BF0A7EEB-B44B-45ED-BC32-7168554FBFCA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="109">
   <si>
     <t>After or During Execution</t>
   </si>
@@ -270,36 +270,171 @@
     <t>User deleted an existing language record</t>
   </si>
   <si>
+    <t>User should not be able to add more records than the minimum of 4</t>
+  </si>
+  <si>
+    <t>User did not add more records than the minimum of 4</t>
+  </si>
+  <si>
+    <t>User should not be able to add a new language record with null data</t>
+  </si>
+  <si>
+    <t>User could not add a new record with null data</t>
+  </si>
+  <si>
+    <t>Verify if the user is able to add a new language record with existing data</t>
+  </si>
+  <si>
+    <t>Verify if the user is able to add a new skill record with existing data</t>
+  </si>
+  <si>
+    <t>User should not be able to add a new record with existing data</t>
+  </si>
+  <si>
+    <t>User could not add a new record with existing data</t>
+  </si>
+  <si>
+    <t>User should be able to add a new language record</t>
+  </si>
+  <si>
+    <t>User should be able to add a new skill record</t>
+  </si>
+  <si>
+    <t>User added a new skill record</t>
+  </si>
+  <si>
+    <t>User should be able to edit an existing skill record</t>
+  </si>
+  <si>
+    <t>User edited an existing skill record</t>
+  </si>
+  <si>
+    <t>User should be able to delete an existing skill record</t>
+  </si>
+  <si>
+    <t>User deleted an existing skill record</t>
+  </si>
+  <si>
+    <t>User should not be able to add a new skill record with null data</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>Verify if the user is able to create a language record using special characters</t>
+  </si>
+  <si>
+    <t>Verify if the user is able to create a skill record using special characters</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Language: !@#$%
+Language Level: Fluent</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>User should not be able to create a language record using special characters</t>
+  </si>
+  <si>
+    <t>User created a language record using special characters</t>
+  </si>
+  <si>
+    <t>User should not be able to create a skill record using special characters</t>
+  </si>
+  <si>
+    <t>User created a skill record using special characters</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Skill: Writing
+Skill Level: Intermediate</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Skill: [null]
+Skill Level: Intermediate</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Skill 1: Writing
+Skill Level 1: Intermediate
+Skill 2: Writing
+Skill Level 2: Intermediate</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Skill: !@#$%
+Skill Level: Intermediate</t>
+  </si>
+  <si>
+    <t>1. Launch "http://localhost:5000/"
+2. Click on "Sign in"
+3. Enter valid credentials
+4. Click on "Login"
+5. Navigate to the "Languages" tab
+6. Click on "Add New"
+7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
+8. Assert the record has been created
+9. Delete the record that was created</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Language: English
+Language Level: Fluent
+Edited Language: Portuguese</t>
+  </si>
+  <si>
+    <t>1. Launch "http://localhost:5000/"
+2. Click on "Sign in"
+3. Enter valid credentials
+4. Click on "Login"
+5. Navigate to the "Languages" tab
+6. Click on "Add New"
+7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
+8. Click on the edit button of the record created
+9. Enter a new language on the text box, click on "Update"
+10. Assert the record has been updated
+11. Delete the record that was updated</t>
+  </si>
+  <si>
+    <t>1. Launch "http://localhost:5000/"
+2. Click on "Sign in"
+3. Enter valid credentials
+4. Click on "Login"
+5. Navigate to the "Languages" tab
+6. Click on "Add New"
+7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
+8. Click on the delete button of the existing record
+9. Assert the record has been deleted</t>
+  </si>
+  <si>
     <t>Email address: leticia.ltm@gmail.com
 Password: QAMars2024*
 Language 1: English
 Language Level 1: Fluent
 Language 2: Portuguese
-Language Level 2: Native/Bilingual
+Language Level 2: Fluent
 Language 3: Spanish
-Language Level 3: Conversational
+Language Level 3: Fluent
 Language 4: French
-Language Level 4: Basic
-Language 5: Italian
-Language Level 5: Basic</t>
-  </si>
-  <si>
-    <t>User should not be able to add more records than the minimum of 4</t>
-  </si>
-  <si>
-    <t>User did not add more records than the minimum of 4</t>
+Language Level 4: Fluent</t>
   </si>
   <si>
     <t>Email address: leticia.ltm@gmail.com
 Password: QAMars2024*
 Language: [null]
-Language Level: Basic</t>
-  </si>
-  <si>
-    <t>User should not be able to add a new language record with null data</t>
-  </si>
-  <si>
-    <t>User could not add a new record with null data</t>
+Language Level: Fluent</t>
   </si>
   <si>
     <t>Email address: leticia.ltm@gmail.com
@@ -307,111 +442,16 @@
 Language 1: English
 Language Level 1: Fluent
 Language 2: English
-Language Level 2: Basic</t>
-  </si>
-  <si>
-    <t>Verify if the user is able to add a new language record with existing data</t>
-  </si>
-  <si>
-    <t>Verify if the user is able to add a new skill record with existing data</t>
-  </si>
-  <si>
-    <t>User should not be able to add a new record with existing data</t>
-  </si>
-  <si>
-    <t>User could not add a new record with existing data</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill: Writing
-Skill Level: Expert</t>
-  </si>
-  <si>
-    <t>User should be able to add a new language record</t>
-  </si>
-  <si>
-    <t>User should be able to add a new skill record</t>
-  </si>
-  <si>
-    <t>User added a new skill record</t>
-  </si>
-  <si>
-    <t>User should be able to edit an existing skill record</t>
-  </si>
-  <si>
-    <t>User edited an existing skill record</t>
-  </si>
-  <si>
-    <t>User should be able to delete an existing skill record</t>
-  </si>
-  <si>
-    <t>User deleted an existing skill record</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill: [null]
-Skill Level: Beginner</t>
-  </si>
-  <si>
-    <t>User should not be able to add a new skill record with null data</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill 1: Writing
-Skill Level 1: Beginner
-Skill 2: Writing
-Skill Level 2: Intermediate</t>
-  </si>
-  <si>
-    <t>TC_014</t>
-  </si>
-  <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>Verify if the user is able to create a language record using special characters</t>
-  </si>
-  <si>
-    <t>Verify if the user is able to create a skill record using special characters</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Language: !@#$%
-Language Level: Fluent</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>User should not be able to create a language record using special characters</t>
-  </si>
-  <si>
-    <t>User created a language record using special characters</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill: !@#$%
-Skill Level: Beginner</t>
-  </si>
-  <si>
-    <t>User should not be able to create a skill record using special characters</t>
-  </si>
-  <si>
-    <t>User created a skill record using special characters</t>
+Language Level 2: Fluent</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
-7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
+7. Type the skill on the text box, click on the dropdown arrow to choose the skill level and click on "Add"
 8. Assert the record has been created
 9. Delete the record that was created</t>
   </si>
@@ -420,158 +460,111 @@
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
 7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
 8. Click on the edit button of the record created
-9. Enter a new language on the text box, click on the dropdown arrow to select a new language level and click on "Update"
+9. Enter a new skill on the text box, click on "Update"
 10. Assert the record has been updated
 11. Delete the record that was updated</t>
+  </si>
+  <si>
+    <t>Email address: leticia.ltm@gmail.com
+Password: QAMars2024*
+Skill: Writing
+Skill Level: Intermediate
+Edit Skill: Photograph</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Languages" tab
 6. Click on "Add New"
 7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
-8. Click on the delete button of the existing record</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Language: Spanish
-Language Level: Basic</t>
+8. Repeat Step 6 &amp; 7
+9. Assert no more records can be added
+10. Delete all the records that were created</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Languages" tab
 6. Click on "Add New"
-7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
-8. Repeat Step 6 &amp; 7 until no more records can't be added
-9. Delete all the records that were created</t>
+7. Type on the text box using special characters, click on the dropdown arrow to choose the language level and click on "Add"
+8. Assert a special characters record is not created
+9. If a record is created, delete the record</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Languages" tab
 6. Click on "Add New"
-7. Type on the text box using special characters, click on the dropdown arrow to choose the language level and click on "Add"
-8. If a record is created, delete the record</t>
+7. Leave the "Add Language" text box empty, click on the dropdown arrow to choose the language level and click on "Add"
+8. Assert a null data record is not created
+9. If a record is created, delete the record</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Languages"
+5. Navigate to the "Languages" tab
 6. Click on "Add New"
-7. Leave the "Add Language" text box empty, click on the dropdown arrow to choose the language level and click on "Add"
-8. If a record is created, delete the record</t>
+7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
+8. Repeat Steps 6 &amp; 7
+9. Assert a duplicate record is not created
+10. Delete all the records that were created</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Skills"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
 7. Type the skill on the text box, click on the dropdown arrow to choose the skill level and click on "Add"
-8. Assert the record has been created
-9. Delete the record that was created</t>
+8. Click on the delete button of the existing record
+9. Assert the record has been deleted</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Skills"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
-7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
-8. Click on the edit button of the record created
-9. Enter a new skill on the text box, click on the dropdown arrow to select a new skill level and click on "Update"
-10. Assert the record has been updated
-11. Delete the record that was updated</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Language: Portuguese
-Language Level: Native/Bilingual
-Edit Language: French
-Edit Language Level: Basic</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill: Constructing
-Skill Level: Intermediate
-Edit Skill: Photograph
-Edit Skill Level: Expert</t>
+7. Leave the "Add Skill" text box empty, click on the dropdown arrow to choose the skill level and click on "Add"
+8. Assert a null data record is not created
+9. If a record is created, delete the record</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Skills"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
 7. Type the skill on the text box, click on the dropdown arrow to choose the skill level and click on "Add"
-8. Click on the delete button of the existing record</t>
-  </si>
-  <si>
-    <t>Email address: leticia.ltm@gmail.com
-Password: QAMars2024*
-Skill: Cooking
-Skill Level: Beginner</t>
+8. Repeat steps 6 &amp; 7
+9. Assert a duplicate record is not created
+10. Delete all the records that were created</t>
   </si>
   <si>
     <t>1. Launch "http://localhost:5000/"
 2. Click on "Sign in"
 3. Enter valid credentials
 4. Click on "Login"
-5. Click on "Profile", then on "Skills"
-6. Click on "Add New"
-7. Leave the "Add Skill" text box empty, click on the dropdown arrow to choose the skill level and click on "Add"
-8. If a record is created, delete the record</t>
-  </si>
-  <si>
-    <t>1. Launch "http://localhost:5000/"
-2. Click on "Sign in"
-3. Enter valid credentials
-4. Click on "Login"
-5. Click on "Profile", then on "Skills"
-6. Click on "Add New"
-7. Type the skill on the text box, click on the dropdown arrow to choose the skill level and click on "Add"
-8. Repeat Steps 6 &amp; 7
-9. Click on the delete button of the existing record</t>
-  </si>
-  <si>
-    <t>1. Launch "http://localhost:5000/"
-2. Click on "Sign in"
-3. Enter valid credentials
-4. Click on "Login"
-5. Click on "Profile", then on "Languages"
-6. Click on "Add New"
-7. Type the language on the text box, click on the dropdown arrow to choose the language level and click on "Add"
-8. Repeat Steps 6 &amp; 7
-9. Click on the delete button of the existing record</t>
-  </si>
-  <si>
-    <t>1. Launch "http://localhost:5000/"
-2. Click on "Sign in"
-3. Enter valid credentials
-4. Click on "Login"
-5. Click on "Profile", then on "Skills"
+5. Navigate to the "Skills" tab
 6. Click on "Add New"
 7. Type on the text box using special characters, click on the dropdown arrow to choose the language level and click on "Add"
-8. If a record is created, delete the record</t>
+8. Assert a special characters record is not created
+9. If a record is created, delete the record</t>
   </si>
 </sst>
 </file>
@@ -1015,9 +1008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308221CA-F4F8-41CE-8DB5-34E24F02B3A3}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,13 +1176,13 @@
         <v>38</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>34</v>
@@ -1213,10 +1206,10 @@
         <v>44</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>45</v>
@@ -1228,7 +1221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="141" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1243,10 +1236,10 @@
         <v>44</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>59</v>
@@ -1258,7 +1251,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="192" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1273,22 +1266,22 @@
         <v>57</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="128.25" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1296,26 +1289,26 @@
         <v>28</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,19 +1326,19 @@
         <v>38</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
@@ -1356,26 +1349,26 @@
         <v>23</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="141" x14ac:dyDescent="0.25">
@@ -1393,22 +1386,22 @@
         <v>38</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="204.75" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="192" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
@@ -1423,22 +1416,22 @@
         <v>58</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="141" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
@@ -1456,19 +1449,19 @@
         <v>105</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="128.25" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="141" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -1483,79 +1476,79 @@
         <v>38</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="128.25" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="153.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>